<commit_message>
changes to ready optimisation
</commit_message>
<xml_diff>
--- a/scripts/data/__params__.xlsx
+++ b/scripts/data/__params__.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/calibrate/optimiser/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C21F112-57C4-40D8-951B-E25FFA3BADE5}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC495868-BF8C-4CB6-9518-B6068ABCA6FF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="45">
   <si>
     <t>Temperature</t>
   </si>
@@ -3999,7 +3999,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I2"/>
+      <selection activeCell="E2" sqref="E2:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4060,59 +4060,6 @@
       </c>
       <c r="C2" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" s="1">
-        <v>327.86500000000001</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.60553000000000001</v>
-      </c>
-      <c r="G2" s="1">
-        <v>81.307000000000002</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>15</v>
-      </c>
-      <c r="J2" s="6">
-        <v>2.1678500999999999E-2</v>
-      </c>
-      <c r="K2" s="6">
-        <v>4.6995700000000001E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="6">
-        <v>20</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1">
-        <v>522.48900000000003</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.2583744</v>
-      </c>
-      <c r="G3" s="1">
-        <v>65.415750000000003</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3.6353333300000002E-5</v>
-      </c>
-      <c r="I3" s="1">
-        <v>15</v>
-      </c>
-      <c r="J3" s="6">
-        <v>7.9900000000000006E-3</v>
-      </c>
-      <c r="K3" s="6">
-        <v>6.3956399999999996E-5</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Major refactoring - see details\n Rewrote the API and restructured the classes (e.g., controller).\n The controller now stores a single instance of the model, instead of creating a model for each curve.\n The user can now define errors for individual curves.\n The user can now modify individual curves (e.g., removing damage), instead of for all the defined curves.\n The user can now define the x and y labels for each error, which minimises the need for repeated errors (e.g., x_end and y_end), as well as allows the user to define errors for curves with more than 2 dimensions (e.g., cyclic) without having to run the model multiple times.\n Implemented the yield strain-stress objective function.\n Implemented a cleaner and simpler print approach.\n Implemented a cleaner recorder for simpler outputs.
</commit_message>
<xml_diff>
--- a/scripts/data/__params__.xlsx
+++ b/scripts/data/__params__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1E1FA6F-FD00-4B38-BD45-58E734A06A41}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36E9FDD2-0CCF-44EE-B7FF-523C27CB95D5}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="3" r:id="rId1"/>
@@ -1366,7 +1366,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1554,7 +1554,7 @@
         <v>9.9885349470504678</v>
       </c>
       <c r="H5" s="1">
-        <v>2.871743109429576</v>
+        <v>2.87174310942958</v>
       </c>
       <c r="I5" s="1">
         <v>9930.2036092384715</v>

</xml_diff>

<commit_message>
Added improved message display for api and fixed damage for non-creep data
</commit_message>
<xml_diff>
--- a/scripts/data/__params__.xlsx
+++ b/scripts/data/__params__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{671724DF-B4D2-4B68-AA3D-5C12FCEA0851}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:1_{95957D69-0AFB-443E-BEFE-75031A2E559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C5C307F-8D72-422D-9B63-AEF2A89761BD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="51">
   <si>
     <t>Temperature</t>
   </si>
@@ -183,12 +183,6 @@
   </si>
   <si>
     <t>A14,16,18,20,F7</t>
-  </si>
-  <si>
-    <t>better creep</t>
-  </si>
-  <si>
-    <t>better tensile</t>
   </si>
 </sst>
 </file>
@@ -864,7 +858,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1373,23 +1367,20 @@
       <c r="C25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="E25" s="1">
-        <v>7.5511999999999997</v>
+        <v>4.8710000000000004</v>
       </c>
       <c r="F25" s="1">
-        <v>23.286000000000001</v>
+        <v>11.518000000000001</v>
       </c>
       <c r="G25" s="1">
-        <v>2.4796</v>
+        <v>7.0281000000000002</v>
       </c>
       <c r="H25" s="1">
-        <v>3.8959000000000001</v>
+        <v>4.2420999999999998</v>
       </c>
       <c r="I25" s="1">
-        <v>1475.4</v>
+        <v>1138.3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1401,9 +1392,6 @@
       </c>
       <c r="C26" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="E26" s="1">
         <v>3.4691999999999998</v>
@@ -2219,8 +2207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283AF620-1FFC-4E74-9A03-F7E60FF34CC2}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>